<commit_message>
adventure stuff and tweaks
</commit_message>
<xml_diff>
--- a/SupersNew/characters/MorphicNanobot.xlsx
+++ b/SupersNew/characters/MorphicNanobot.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="264">
   <si>
     <t>Name</t>
   </si>
@@ -669,13 +669,629 @@
   </si>
   <si>
     <t>Morphic Nanobot</t>
+  </si>
+  <si>
+    <t>Nanobot/insect Form</t>
+  </si>
+  <si>
+    <t>360 Degree Vision</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Can see in all directions</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cannot be flanked</t>
+    </r>
+  </si>
+  <si>
+    <t>Carapace</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Armor 4/2/0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Move -1</t>
+    </r>
+  </si>
+  <si>
+    <t>Clinging</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Can cling to walls, ceilings, etc.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Muscle +8 with grabs and holds</t>
+    </r>
+  </si>
+  <si>
+    <t>Venom</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Envenomed (Toughness)</t>
+    </r>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>Ars</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>4/</t>
+  </si>
+  <si>
+    <t>1 tgt</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Armor 0/0/0 &amp; 4d8 Entangle</t>
+    </r>
+  </si>
+  <si>
+    <t>Nano Armor</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Armor 3/3/0</t>
+    </r>
+  </si>
+  <si>
+    <t>Adaptive Armor</t>
+  </si>
+  <si>
+    <t>R+</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Any armor you have can be shifted between physical and energy armor</t>
+    </r>
+  </si>
+  <si>
+    <t>Omni Arm</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Can turn your arms/hands into tools</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Cannot create power for power tools </t>
+    </r>
+  </si>
+  <si>
+    <t>M/U</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Can use Muscle at 8 hex range</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Can move up to 8 hexes as a move action</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Must end your move on a surface, or hanging onto something</t>
+    </r>
+  </si>
+  <si>
+    <t>Nano Blade</t>
+  </si>
+  <si>
+    <t>Amt</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>3d6 Physical Stab Damage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>You can sacrifice any armor you have until the beginning of your next action to gain a damage boost of (Armor/2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Knock(0)</t>
+    </r>
+  </si>
+  <si>
+    <t>Extrude</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Can extrude through small openings</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Can escape grapples with +10 Muscle</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Can escape from any entangle with gaps</t>
+    </r>
+  </si>
+  <si>
+    <t>Machine Interface</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Proficient in Computer, Electronics or using vehicles/tools with such parts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Abadi"/>
+        <family val="2"/>
+      </rPr>
+      <t>Skill +4</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -710,6 +1326,25 @@
       <name val="Century Gothic"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Abadi"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -731,7 +1366,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -780,11 +1415,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -821,6 +1552,54 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1136,10 +1915,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection sqref="A1:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,7 +1957,9 @@
       <c r="A2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="17" t="s">
+        <v>212</v>
+      </c>
       <c r="C2" s="17"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
@@ -1251,11 +2035,11 @@
         <v>9</v>
       </c>
       <c r="B7" s="8">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" ref="C7:C13" si="0">(B7 - 10)/2</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
@@ -1263,7 +2047,7 @@
       </c>
       <c r="F7" s="4">
         <f>_xlfn.FLOOR.MATH(VLOOKUP(G2,'Fighting Profiles'!A2:F48,2,FALSE))</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -1273,11 +2057,11 @@
         <v>8</v>
       </c>
       <c r="B8" s="8">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
@@ -1285,7 +2069,7 @@
       </c>
       <c r="F8" s="4">
         <f>_xlfn.FLOOR.MATH(VLOOKUP(G2,'Fighting Profiles'!A2:F48,3,FALSE))</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -1295,11 +2079,11 @@
         <v>15</v>
       </c>
       <c r="B9" s="8">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
@@ -1307,7 +2091,7 @@
       </c>
       <c r="F9" s="4">
         <f>_xlfn.FLOOR.MATH(VLOOKUP(G2,'Fighting Profiles'!A2:F48,4,FALSE))</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -1317,11 +2101,11 @@
         <v>16</v>
       </c>
       <c r="B10" s="8">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
@@ -1329,7 +2113,7 @@
       </c>
       <c r="F10" s="4">
         <f>_xlfn.FLOOR.MATH(VLOOKUP(G2,'Fighting Profiles'!A2:F48,5,FALSE))</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -1339,11 +2123,11 @@
         <v>17</v>
       </c>
       <c r="B11" s="8">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
@@ -1351,7 +2135,7 @@
       </c>
       <c r="F11" s="4">
         <f>_xlfn.FLOOR.MATH(VLOOKUP(G2,'Fighting Profiles'!A2:F48,6,FALSE))</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -1361,11 +2145,11 @@
         <v>18</v>
       </c>
       <c r="B12" s="8">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1378,11 +2162,11 @@
         <v>19</v>
       </c>
       <c r="B13" s="8">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -1406,7 +2190,7 @@
       </c>
       <c r="B15" s="4">
         <f>_xlfn.CEILING.MATH($B$7*0.5) + _xlfn.CEILING.MATH($B$12 *0.5) + $B$10 + 8</f>
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="7" t="s">
@@ -1424,7 +2208,7 @@
         <v>73</v>
       </c>
       <c r="B16" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1439,7 +2223,7 @@
       </c>
       <c r="B17" s="4">
         <f xml:space="preserve"> _xlfn.FLOOR.MATH(C11+C9)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1471,7 +2255,7 @@
       <c r="H19" s="7"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>0</v>
       </c>
@@ -1500,26 +2284,556 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="D21" s="23">
+        <v>10</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="H21" s="23">
+        <v>0</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="22" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="D23" s="23">
+        <v>20</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="H23" s="23">
+        <v>0</v>
+      </c>
+      <c r="I23" s="21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="22" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="D25" s="23">
+        <v>20</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="H25" s="23">
+        <v>0</v>
+      </c>
+      <c r="I25" s="27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="22" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>228</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="D27" s="30">
+        <v>20</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="F27" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="G27" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="H27" s="30">
+        <v>2</v>
+      </c>
+      <c r="I27" s="32" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="33" t="s">
+        <v>231</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="D28" s="34">
+        <v>20</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="F28" s="34">
+        <v>0</v>
+      </c>
+      <c r="G28" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="H28" s="34">
+        <v>4</v>
+      </c>
+      <c r="I28" s="22" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="D29" s="30">
+        <v>20</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="G29" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="H29" s="30">
+        <v>0</v>
+      </c>
+      <c r="I29" s="32" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="D30" s="30">
+        <v>30</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="F30" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="H30" s="30">
+        <v>4</v>
+      </c>
+      <c r="I30" s="32" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="D31" s="23">
+        <v>10</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="G31" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="I31" s="21" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="22" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>247</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="D33" s="23">
+        <v>20</v>
+      </c>
+      <c r="E33" s="23">
+        <v>12</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="H33" s="23">
+        <v>1</v>
+      </c>
+      <c r="I33" s="27" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A34" s="28"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="27" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="24"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="22" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="D36" s="23">
+        <v>20</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="F36" s="23">
+        <v>0</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="H36" s="23">
+        <v>4</v>
+      </c>
+      <c r="I36" s="21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+      <c r="A37" s="28"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="27" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="24"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="22" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A39" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="D39" s="23">
+        <v>20</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="H39" s="23">
+        <v>4</v>
+      </c>
+      <c r="I39" s="21" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A40" s="28"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="27" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="24"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A42" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="27" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="24"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="22" t="s">
+        <v>263</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="68">
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="H39:H41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="G36:G38"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="H33:H35"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
     <mergeCell ref="G16:G18"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="E15:F15"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="67" fitToWidth="0" orientation="landscape" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1533,7 +2847,7 @@
           <x14:formula1>
             <xm:f>'Power Sets'!$A$2:$A$48</xm:f>
           </x14:formula1>
-          <xm:sqref>B3 C3</xm:sqref>
+          <xm:sqref>B3:C3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1545,7 +2859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1851,23 +3165,23 @@
       </c>
       <c r="B2" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D2" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E2" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F2" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C11+2+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1879,23 +3193,23 @@
       </c>
       <c r="B3" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C11+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C3" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D3" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E3" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F3" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C11+1+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -1909,23 +3223,23 @@
       </c>
       <c r="B4" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C8+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D4" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C11+1+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E4" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C8+0+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F4" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+3+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -1939,23 +3253,23 @@
       </c>
       <c r="B5" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+1+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D5" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+4+8</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E5" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F5" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C12+0+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -1969,23 +3283,23 @@
       </c>
       <c r="B6" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+5+8</f>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D6" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C7+1+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E6" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F6" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C10+'Character Sheet'!C12+0+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -1999,23 +3313,23 @@
       </c>
       <c r="B7" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+1+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C7" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+1+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D7" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C12+4+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E7" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F7" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+1+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -2029,23 +3343,23 @@
       </c>
       <c r="B8" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C8" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C10+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D8" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E8" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F8" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C10+'Character Sheet'!C12+1+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -2059,23 +3373,23 @@
       </c>
       <c r="B9" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+2+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C8+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D9" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C9+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E9" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F9" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+1+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -2089,23 +3403,23 @@
       </c>
       <c r="B10" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+4+8</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C10" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D10" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E10" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F10" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+0+8</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -2117,23 +3431,23 @@
       </c>
       <c r="B11" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+4+8</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C11" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C8+'Character Sheet'!C10+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D11" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E11" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F11" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C10+'Character Sheet'!C12+1+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -2147,23 +3461,23 @@
       </c>
       <c r="B12" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C11+0+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C12" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D12" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C9+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E12" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F12" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C12+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -2177,23 +3491,23 @@
       </c>
       <c r="B13" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C13" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D13" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C9+4+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E13" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F13" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C13+0+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -2207,23 +3521,23 @@
       </c>
       <c r="B14" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C14" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C10+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D14" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E14" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+1+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F14" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C10+'Character Sheet'!C12+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -2237,23 +3551,23 @@
       </c>
       <c r="B15" s="11">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C9+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C15" s="11">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+0+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D15" s="11">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E15" s="11">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F15" s="11">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C13+3+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -2267,23 +3581,23 @@
       </c>
       <c r="B16" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C8+0+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C16" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C9+1+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D16" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+1+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E16" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C11+3+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F16" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+5+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -2297,23 +3611,23 @@
       </c>
       <c r="B17" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C11+1+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C17" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D17" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E17" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F17" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C13+2+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -2327,23 +3641,23 @@
       </c>
       <c r="B18" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C9+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C18" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D18" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E18" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F18" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+0+8</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -2355,23 +3669,23 @@
       </c>
       <c r="B19" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C19" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D19" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E19" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C8+'Character Sheet'!C9+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F19" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+0+8</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -2385,23 +3699,23 @@
       </c>
       <c r="B20" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+4+8</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C20" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+4+8</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D20" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+0+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E20" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F20" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+0+8</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -2415,23 +3729,23 @@
       </c>
       <c r="B21" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C7+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C21" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D21" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E21" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F21" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+2+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -2445,23 +3759,23 @@
       </c>
       <c r="B22" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C9+4+8</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C22" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+1+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D22" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+1+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E22" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F22" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+1+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -2475,23 +3789,23 @@
       </c>
       <c r="B23" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C23" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D23" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E23" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F23" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C10+'Character Sheet'!C12+0+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -2505,23 +3819,23 @@
       </c>
       <c r="B24" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C24" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C10+4+8</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D24" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+0+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E24" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C10+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F24" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C10+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -2535,23 +3849,23 @@
       </c>
       <c r="B25" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C13+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C25" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C8+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D25" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C9+0+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E25" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F25" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+2+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -2565,23 +3879,23 @@
       </c>
       <c r="B26" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C13+2+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C26" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D26" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+2+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E26" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F26" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C13+2+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -2593,23 +3907,23 @@
       </c>
       <c r="B27" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C7+0+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C27" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D27" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E27" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F27" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+2+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -2623,23 +3937,23 @@
       </c>
       <c r="B28" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C28" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D28" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+1+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E28" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F28" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C11+1+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -2653,23 +3967,23 @@
       </c>
       <c r="B29" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+0+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C29" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+1+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D29" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E29" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F29" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C11+4+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
@@ -2683,23 +3997,23 @@
       </c>
       <c r="B30" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C30" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D30" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+1+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E30" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+4+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F30" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C9+0+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
@@ -2713,23 +4027,23 @@
       </c>
       <c r="B31" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C31" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C10+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D31" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E31" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C10+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F31" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C10+'Character Sheet'!C11+0+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
@@ -2743,23 +4057,23 @@
       </c>
       <c r="B32" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+0+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C32" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+1+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D32" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E32" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F32" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C13+3+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -2773,23 +4087,23 @@
       </c>
       <c r="B33" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C12+0+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C33" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C8+1+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D33" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+1+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E33" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C9+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F33" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+5+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -2803,23 +4117,23 @@
       </c>
       <c r="B34" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C34" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C12+4+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D34" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C8+1+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E34" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F34" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C13+0+8</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -2831,23 +4145,23 @@
       </c>
       <c r="B35" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C9+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C35" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C8+'Character Sheet'!C9+0+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D35" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C9+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E35" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C12+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F35" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+3+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
@@ -2861,23 +4175,23 @@
       </c>
       <c r="B36" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+0+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C36" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+1+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D36" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C8+5+8</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E36" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C12+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F36" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+0+8</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
@@ -2891,23 +4205,23 @@
       </c>
       <c r="B37" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C37" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D37" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E37" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F37" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+0+8</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
@@ -2921,23 +4235,23 @@
       </c>
       <c r="B38" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C9+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C38" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+1+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D38" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+1+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E38" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+5+8</f>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F38" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C13+0+8</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
@@ -2951,23 +4265,23 @@
       </c>
       <c r="B39" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+0+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C39" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D39" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C8+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E39" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F39" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+3+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -2981,23 +4295,23 @@
       </c>
       <c r="B40" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C8+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C40" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C10+'Character Sheet'!C12+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D40" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C8+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E40" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C12+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F40" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C9+0+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
@@ -3011,23 +4325,23 @@
       </c>
       <c r="B41" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C12+0+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C41" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D41" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C8+4+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E41" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C12+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F41" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+2+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
@@ -3041,23 +4355,23 @@
       </c>
       <c r="B42" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C9+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C42" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+0+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D42" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+4+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E42" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F42" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+1+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
@@ -3069,23 +4383,23 @@
       </c>
       <c r="B43" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+0+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C43" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D43" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C8+'Character Sheet'!C12+4+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E43" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F43" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+1+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
@@ -3099,23 +4413,23 @@
       </c>
       <c r="B44" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C12+4+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C44" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C10+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D44" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C12+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E44" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C10+0+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F44" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+0+8</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
@@ -3129,23 +4443,23 @@
       </c>
       <c r="B45" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C45" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D45" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+1+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E45" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C2+'Character Sheet'!C8+2+8</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F45" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+1+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
@@ -3159,23 +4473,23 @@
       </c>
       <c r="B46" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C9+1+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C46" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D46" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E46" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C9+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F46" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C13+2+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
@@ -3189,23 +4503,23 @@
       </c>
       <c r="B47" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C47" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C10+3+8</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D47" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E47" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F47" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C10+'Character Sheet'!C12+0+8</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
@@ -3219,23 +4533,23 @@
       </c>
       <c r="B48" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C11+1+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C48" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C8+'Character Sheet'!C9+2+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D48" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C9+2+8</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E48" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+3+8</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F48" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C13+2+8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>

</xml_diff>